<commit_message>
Updated base URL on all pages, we need to follow the it is implemented currently. DO NOT hard code the url in the PageObject
</commit_message>
<xml_diff>
--- a/Automation/src/com/heal/framework/test/Run.xlsx
+++ b/Automation/src/com/heal/framework/test/Run.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahanmelikyan/Documents/workspace/heal-qa-automation/Automation/src/com/heal/framework/test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4778" yWindow="1238" windowWidth="28823" windowHeight="14543" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6260" yWindow="1240" windowWidth="28820" windowHeight="14540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Configs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Execute</t>
   </si>
@@ -126,69 +131,85 @@
     <t>macOS 10.12</t>
   </si>
   <si>
+    <t>loginWithValidCredentials</t>
+  </si>
+  <si>
+    <t>bookVisitWithCreditCard</t>
+  </si>
+  <si>
+    <t>patient.tests.VisitTest</t>
+  </si>
+  <si>
+    <t>BookVisitWithInsurance</t>
+  </si>
+  <si>
+    <t>BookVisitWith100PercentPromo</t>
+  </si>
+  <si>
+    <t>BookVisitWith50PercentPromo</t>
+  </si>
+  <si>
+    <t>cancelVisit</t>
+  </si>
+  <si>
+    <t>editProfile</t>
+  </si>
+  <si>
+    <t>patient.tests.PaymentsTest</t>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>retryLimit</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>patient.tests.LoginTest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>baseUrl</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>loginWithValidCredentials</t>
-  </si>
-  <si>
-    <t>bookVisitWithCreditCard</t>
-  </si>
-  <si>
-    <t>patient.tests.VisitTest</t>
-  </si>
-  <si>
-    <t>BookVisitWithInsurance</t>
-  </si>
-  <si>
-    <t>BookVisitWith100PercentPromo</t>
-  </si>
-  <si>
-    <t>BookVisitWith50PercentPromo</t>
-  </si>
-  <si>
-    <t>cancelVisit</t>
-  </si>
-  <si>
-    <t>editProfile</t>
-  </si>
-  <si>
-    <t>patient.tests.PaymentsTest</t>
-  </si>
-  <si>
-    <t>patient.qa.heal.com</t>
-  </si>
-  <si>
-    <t>N</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>retryLimit</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>patient.tests.LoginTest</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>.qa.heal.com</t>
+  </si>
+  <si>
+    <t>-dev.heal.com</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environment </t>
+  </si>
+  <si>
+    <t>PROD</t>
+  </si>
+  <si>
+    <t>URLs</t>
+  </si>
+  <si>
+    <t>doNotRunInPROD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -203,13 +224,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -218,7 +239,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -226,24 +247,57 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="DengXian"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -273,28 +327,105 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="已访问的超链接" xfId="1" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="2" builtinId="8" hidden="1"/>
+  <cellStyles count="8">
+    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -593,23 +724,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A12"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.46484375" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="36.1328125" customWidth="1"/>
+    <col min="5" max="5" width="36.1640625" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.65" thickBot="1">
+    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,43 +760,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
       <c r="D2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -674,20 +805,20 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -696,59 +827,59 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -762,123 +893,208 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.9"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.1328125" style="3"/>
+    <col min="1" max="1" width="32.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="8" t="str">
+        <f>IF(B8="QA",Configs!B2,IF(B8="DEV",Configs!B3,IF(B8="PROD",Configs!B4,"")))</f>
+        <v>.qa.heal.com</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>44</v>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="A8:B8">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="DEV">
+      <formula>NOT(ISERROR(SEARCH("DEV",A8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="QA">
+      <formula>NOT(ISERROR(SEARCH("QA",B8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="PROD">
+      <formula>NOT(ISERROR(SEARCH("PROD",B8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="doNotRunInPROD">
+      <formula>NOT(ISERROR(SEARCH("doNotRunInPROD",B7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
+      <formula1>0</formula1>
+      <formula2>5</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Configs!$A$2:$A$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>B8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added a selection for different environments.
</commit_message>
<xml_diff>
--- a/Automation/src/com/heal/framework/test/Run.xlsx
+++ b/Automation/src/com/heal/framework/test/Run.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="1240" windowWidth="28820" windowHeight="14540" activeTab="1"/>
+    <workbookView xWindow="6720" yWindow="1380" windowWidth="28820" windowHeight="14540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>Execute</t>
   </si>
@@ -158,47 +158,52 @@
     <t>patient.tests.PaymentsTest</t>
   </si>
   <si>
+    <t>Y</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>retryLimit</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>patient.tests.LoginTest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseUrl</t>
+  </si>
+  <si>
+    <t>.qa.heal.com</t>
+  </si>
+  <si>
+    <t>-dev.heal.com</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environment </t>
+  </si>
+  <si>
+    <t>PROD</t>
+  </si>
+  <si>
+    <t>URLs</t>
+  </si>
+  <si>
+    <t>doNotRunInPROD</t>
+  </si>
+  <si>
     <t>N</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>retryLimit</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>patient.tests.LoginTest</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>baseUrl</t>
-  </si>
-  <si>
-    <t>.qa.heal.com</t>
-  </si>
-  <si>
-    <t>-dev.heal.com</t>
-  </si>
-  <si>
-    <t>DEV</t>
-  </si>
-  <si>
-    <t>QA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Environment </t>
-  </si>
-  <si>
-    <t>PROD</t>
-  </si>
-  <si>
-    <t>URLs</t>
-  </si>
-  <si>
-    <t>doNotRunInPROD</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -337,22 +342,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -364,7 +364,7 @@
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
       <font>
         <b/>
@@ -385,7 +385,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -398,18 +398,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -728,7 +716,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -762,10 +750,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
@@ -773,7 +761,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
@@ -897,22 +885,22 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" style="3" customWidth="1"/>
     <col min="4" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
@@ -925,42 +913,42 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="8" t="str">
+      <c r="A7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="5" t="str">
         <f>IF(B8="QA",Configs!B2,IF(B8="DEV",Configs!B3,IF(B8="PROD",Configs!B4,"")))</f>
         <v>.qa.heal.com</v>
       </c>
@@ -968,69 +956,65 @@
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="10" t="s">
-        <v>47</v>
+      <c r="A8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="9">
-        <v>1</v>
+      <c r="A12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A8:B8">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="DEV">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="DEV">
       <formula>NOT(ISERROR(SEARCH("DEV",A8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="QA">
-      <formula>NOT(ISERROR(SEARCH("QA",B8)))</formula>
-    </cfRule>
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="PROD">
       <formula>NOT(ISERROR(SEARCH("PROD",B8)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="QA">
+      <formula>NOT(ISERROR(SEARCH("QA",B8)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="doNotRunInPROD">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="doNotRunInPROD">
       <formula>NOT(ISERROR(SEARCH("doNotRunInPROD",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
-      <formula1>0</formula1>
-      <formula2>5</formula2>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -1064,34 +1048,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed excel empty rows issue
</commit_message>
<xml_diff>
--- a/Automation/src/com/heal/framework/test/Run.xlsx
+++ b/Automation/src/com/heal/framework/test/Run.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>Execute</t>
   </si>
@@ -166,39 +166,47 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>patient.tests.LoginTest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseUrl</t>
+  </si>
+  <si>
+    <t>.qa.heal.com</t>
+  </si>
+  <si>
+    <t>-dev.heal.com</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environment </t>
+  </si>
+  <si>
+    <t>PROD</t>
+  </si>
+  <si>
+    <t>URLs</t>
+  </si>
+  <si>
+    <t>doNotRunInPROD</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>retryLimit</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>patient.tests.LoginTest</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>baseUrl</t>
-  </si>
-  <si>
-    <t>.qa.heal.com</t>
-  </si>
-  <si>
-    <t>-dev.heal.com</t>
-  </si>
-  <si>
-    <t>DEV</t>
-  </si>
-  <si>
-    <t>QA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Environment </t>
-  </si>
-  <si>
-    <t>PROD</t>
-  </si>
-  <si>
-    <t>URLs</t>
-  </si>
-  <si>
-    <t>doNotRunInPROD</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ENV</t>
   </si>
 </sst>
 </file>
@@ -337,22 +345,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -364,7 +368,7 @@
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
       <font>
         <b/>
@@ -385,7 +389,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor theme="6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -398,18 +402,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -728,7 +720,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A4" sqref="A4:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -765,7 +757,7 @@
         <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
@@ -785,7 +777,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -796,7 +788,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -807,7 +799,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -818,7 +810,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -829,7 +821,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
@@ -840,7 +832,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
         <v>32</v>
@@ -851,7 +843,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
         <v>32</v>
@@ -862,7 +854,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
@@ -873,7 +865,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
         <v>32</v>
@@ -894,7 +886,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -902,65 +894,65 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" style="3" customWidth="1"/>
     <col min="4" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="8" t="str">
+      <c r="A7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="5" t="str">
         <f>IF(B8="QA",Configs!B2,IF(B8="DEV",Configs!B3,IF(B8="PROD",Configs!B4,"")))</f>
         <v>.qa.heal.com</v>
       </c>
@@ -968,69 +960,164 @@
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="10" t="s">
-        <v>47</v>
+      <c r="A8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="9">
-        <v>1</v>
-      </c>
+      <c r="A12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A8:B8">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="DEV">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="DEV">
       <formula>NOT(ISERROR(SEARCH("DEV",A8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="QA">
-      <formula>NOT(ISERROR(SEARCH("QA",B8)))</formula>
-    </cfRule>
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="PROD">
       <formula>NOT(ISERROR(SEARCH("PROD",B8)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="QA">
+      <formula>NOT(ISERROR(SEARCH("QA",B8)))</formula>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="doNotRunInPROD">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="doNotRunInPROD">
       <formula>NOT(ISERROR(SEARCH("doNotRunInPROD",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
-      <formula1>0</formula1>
-      <formula2>5</formula2>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -1064,34 +1151,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
to support run tests on saucelabs
</commit_message>
<xml_diff>
--- a/Automation/src/com/heal/framework/test/Run.xlsx
+++ b/Automation/src/com/heal/framework/test/Run.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahanmelikyan/Documents/workspace/heal-qa-automation/Automation/src/com/heal/framework/test/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="1240" windowWidth="28820" windowHeight="14540" activeTab="1"/>
+    <workbookView xWindow="6263" yWindow="1238" windowWidth="28823" windowHeight="14543" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="4" r:id="rId2"/>
     <sheet name="Configs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>Execute</t>
   </si>
@@ -116,21 +111,12 @@
     <t>@ondemand.saucelabs.com:443/wd/hub</t>
   </si>
   <si>
-    <t>local</t>
-  </si>
-  <si>
     <t>editPayments</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
     <t>addProfile</t>
   </si>
   <si>
-    <t>macOS 10.12</t>
-  </si>
-  <si>
     <t>loginWithValidCredentials</t>
   </si>
   <si>
@@ -197,9 +183,6 @@
     <t>doNotRunInPROD</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>retryLimit</t>
   </si>
   <si>
@@ -207,17 +190,69 @@
   </si>
   <si>
     <t>ENV</t>
+  </si>
+  <si>
+    <t>remote</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>appiumVersion</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>deviceName</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>deviceOrientation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>platformVersion</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>platformName</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.6.4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>iPhone 7 Simulator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>portrait</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>iOS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>iphone</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Safari</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -232,13 +267,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -247,7 +282,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -255,21 +290,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -277,7 +312,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -359,14 +394,14 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -716,23 +751,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A12"/>
+      <selection activeCell="A3" sqref="A3:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="10.46484375" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="36.1640625" customWidth="1"/>
+    <col min="5" max="5" width="36.1328125" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -752,20 +787,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
@@ -775,42 +810,42 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -819,59 +854,59 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -885,22 +920,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.9"/>
   <cols>
     <col min="1" max="1" width="32.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.1640625" style="3"/>
+    <col min="3" max="3" width="12.1328125" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -908,31 +943,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -940,7 +975,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -948,9 +983,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B7" s="5" t="str">
         <f>IF(B8="QA",Configs!B2,IF(B8="DEV",Configs!B3,IF(B8="PROD",Configs!B4,"")))</f>
@@ -959,15 +994,15 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -975,7 +1010,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -983,7 +1018,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
@@ -991,112 +1026,140 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44" s="3"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1">
       <c r="A45" s="3"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1123,7 +1186,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Configs!$A$2:$A$10</xm:f>
           </x14:formula1>
@@ -1136,49 +1199,49 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
         <v>47</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resetPassword test and some adjustments
</commit_message>
<xml_diff>
--- a/Automation/src/com/heal/framework/test/Run.xlsx
+++ b/Automation/src/com/heal/framework/test/Run.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
   <si>
     <t>Execute</t>
   </si>
@@ -158,10 +158,6 @@
     <t>patient.tests.PaymentsTest</t>
   </si>
   <si>
-    <t>N</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>patient.tests.LoginTest</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -208,13 +204,56 @@
     <t>ops.tests.LoginTest</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>checkDashboardElements</t>
   </si>
   <si>
     <t>ops.tests.DashboardTest</t>
+  </si>
+  <si>
+    <t>appiumVersion</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.6.4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>deviceName</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>iPhone 7 Simulator</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>deviceOrientation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>portrait</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>platformVersion</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>platformName</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>iOS</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>patient.tests.PasswordTest</t>
+  </si>
+  <si>
+    <t>resetPassword</t>
   </si>
 </sst>
 </file>
@@ -725,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -762,10 +801,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
@@ -773,7 +812,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
@@ -785,7 +824,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
@@ -796,7 +835,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -807,7 +846,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -818,7 +857,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -829,7 +868,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
@@ -840,7 +879,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
         <v>32</v>
@@ -851,7 +890,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
         <v>32</v>
@@ -862,7 +901,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
@@ -873,7 +912,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>32</v>
@@ -884,24 +923,35 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -919,7 +969,7 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A14" sqref="A14:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -980,7 +1030,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="5" t="str">
         <f>IF(B8="QA",Configs!B2,IF(B8="DEV",Configs!B3,IF(B8="PROD",Configs!B4,"")))</f>
@@ -991,10 +1041,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1023,70 +1073,95 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
+      <c r="A14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
@@ -1181,34 +1256,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>